<commit_message>
Adds rock weathering to WebAppData, updates ERWD to EU data
</commit_message>
<xml_diff>
--- a/InputData/geoeng/ERWD/Enhanced Rock Weathering Data.xlsx
+++ b/InputData/geoeng/ERWD/Enhanced Rock Weathering Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\geoeng\ERWD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\geoeng\ERWD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AAF143-D02D-4BA9-A61C-1E4CE8806B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13A63CE-058B-4FF2-80E7-6316106B699D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58455" yWindow="2640" windowWidth="19830" windowHeight="13320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -138,12 +138,6 @@
     <t>Supplemental information, Figure 9</t>
   </si>
   <si>
-    <t>We report the US specific cost and potential.</t>
-  </si>
-  <si>
-    <t>USA representative cost per ton</t>
-  </si>
-  <si>
     <t>Total potential</t>
   </si>
   <si>
@@ -178,6 +172,12 @@
   </si>
   <si>
     <t>a very large scale-up of capacity and transportation logistics.</t>
+  </si>
+  <si>
+    <t>We report the EU specific cost and potential.</t>
+  </si>
+  <si>
+    <t>EU representative cost per ton</t>
   </si>
 </sst>
 </file>
@@ -297,8 +297,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>438945</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>181556</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>581</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -599,32 +599,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" customWidth="1"/>
     <col min="2" max="2" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,89 +632,89 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="5">
         <v>2023</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0.88711067149387013</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>947817</v>
@@ -731,51 +731,52 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="4" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" customWidth="1"/>
+    <col min="4" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <f>268+402</f>
+        <v>670</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>0.66</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
     </row>
   </sheetData>
@@ -792,19 +793,19 @@
   </sheetPr>
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="32" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="21" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="32" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -902,7 +903,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -924,107 +925,107 @@
       </c>
       <c r="G2" s="8" cm="1">
         <f t="array" ref="G2">TREND($L$2-$F$2)/COUNT($G$1:$L$1)+F2</f>
-        <v>116666666.66666667</v>
+        <v>111666666.66666667</v>
       </c>
       <c r="H2" s="8" cm="1">
         <f t="array" ref="H2">TREND($L$2-$F$2)/COUNT($G$1:$L$1)+G2</f>
-        <v>233333333.33333334</v>
+        <v>223333333.33333334</v>
       </c>
       <c r="I2" s="8" cm="1">
         <f t="array" ref="I2">TREND($L$2-$F$2)/COUNT($G$1:$L$1)+H2</f>
-        <v>350000000</v>
+        <v>335000000</v>
       </c>
       <c r="J2" s="8" cm="1">
         <f t="array" ref="J2">TREND($L$2-$F$2)/COUNT($G$1:$L$1)+I2</f>
-        <v>466666666.66666669</v>
+        <v>446666666.66666669</v>
       </c>
       <c r="K2" s="8" cm="1">
         <f t="array" ref="K2">TREND($L$2-$F$2)/COUNT($G$1:$L$1)+J2</f>
-        <v>583333333.33333337</v>
+        <v>558333333.33333337</v>
       </c>
       <c r="L2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="M2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="N2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="O2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="P2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="Q2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="R2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="S2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="T2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="U2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="V2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="W2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="X2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="Y2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="Z2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="AA2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="AB2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="AC2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="AD2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="AE2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
       <c r="AF2" s="8">
         <f>'Fuhrman data'!$B$3*10^6</f>
-        <v>700000000</v>
+        <v>670000000</v>
       </c>
     </row>
   </sheetData>
@@ -1043,12 +1044,12 @@
       <selection activeCell="C2" sqref="C2:AF2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1146,7 +1147,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1275,7 +1276,7 @@
         <v>625559.22</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1373,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1471,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1569,7 +1570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1667,7 +1668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1765,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1863,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1961,7 +1962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2059,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2173,12 +2174,12 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2276,133 +2277,133 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
         <f>('Fuhrman data'!B1+'Fuhrman data'!B2)*About!A25</f>
-        <v>255.4878733902346</v>
+        <v>299.84340696492808</v>
       </c>
       <c r="C2">
         <f>($AF$2-$B$2)/COUNT($C$1:$AF$1)+B2</f>
-        <v>251.4071643013628</v>
+        <v>295.76269787605628</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:AE2" si="0">($AF$2-$B$2)/COUNT($C$1:$AF$1)+C2</f>
-        <v>247.326455212491</v>
+        <v>291.68198878718448</v>
       </c>
       <c r="E2">
         <f t="shared" si="0"/>
-        <v>243.2457461236192</v>
+        <v>287.60127969831268</v>
       </c>
       <c r="F2">
         <f t="shared" si="0"/>
-        <v>239.1650370347474</v>
+        <v>283.52057060944088</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
-        <v>235.0843279458756</v>
+        <v>279.43986152056908</v>
       </c>
       <c r="H2">
         <f t="shared" si="0"/>
-        <v>231.0036188570038</v>
+        <v>275.35915243169728</v>
       </c>
       <c r="I2">
         <f t="shared" si="0"/>
-        <v>226.922909768132</v>
+        <v>271.27844334282548</v>
       </c>
       <c r="J2">
         <f t="shared" si="0"/>
-        <v>222.8422006792602</v>
+        <v>267.19773425395368</v>
       </c>
       <c r="K2">
         <f t="shared" si="0"/>
-        <v>218.7614915903884</v>
+        <v>263.11702516508188</v>
       </c>
       <c r="L2">
         <f t="shared" si="0"/>
-        <v>214.6807825015166</v>
+        <v>259.03631607621008</v>
       </c>
       <c r="M2">
         <f t="shared" si="0"/>
-        <v>210.6000734126448</v>
+        <v>254.95560698733829</v>
       </c>
       <c r="N2">
         <f t="shared" si="0"/>
-        <v>206.519364323773</v>
+        <v>250.87489789846649</v>
       </c>
       <c r="O2">
         <f t="shared" si="0"/>
-        <v>202.4386552349012</v>
+        <v>246.79418880959469</v>
       </c>
       <c r="P2">
         <f t="shared" si="0"/>
-        <v>198.35794614602941</v>
+        <v>242.71347972072289</v>
       </c>
       <c r="Q2">
         <f t="shared" si="0"/>
-        <v>194.27723705715761</v>
+        <v>238.63277063185109</v>
       </c>
       <c r="R2">
         <f t="shared" si="0"/>
-        <v>190.19652796828581</v>
+        <v>234.55206154297929</v>
       </c>
       <c r="S2">
         <f t="shared" si="0"/>
-        <v>186.11581887941401</v>
+        <v>230.47135245410749</v>
       </c>
       <c r="T2">
         <f t="shared" si="0"/>
-        <v>182.03510979054221</v>
+        <v>226.39064336523569</v>
       </c>
       <c r="U2">
         <f t="shared" si="0"/>
-        <v>177.95440070167041</v>
+        <v>222.30993427636389</v>
       </c>
       <c r="V2">
         <f t="shared" si="0"/>
-        <v>173.87369161279861</v>
+        <v>218.22922518749209</v>
       </c>
       <c r="W2">
         <f t="shared" si="0"/>
-        <v>169.79298252392681</v>
+        <v>214.14851609862029</v>
       </c>
       <c r="X2">
         <f t="shared" si="0"/>
-        <v>165.71227343505501</v>
+        <v>210.06780700974849</v>
       </c>
       <c r="Y2">
         <f t="shared" si="0"/>
-        <v>161.63156434618321</v>
+        <v>205.98709792087669</v>
       </c>
       <c r="Z2">
         <f t="shared" si="0"/>
-        <v>157.55085525731141</v>
+        <v>201.90638883200489</v>
       </c>
       <c r="AA2">
         <f t="shared" si="0"/>
-        <v>153.47014616843961</v>
+        <v>197.82567974313309</v>
       </c>
       <c r="AB2">
         <f t="shared" si="0"/>
-        <v>149.38943707956781</v>
+        <v>193.74497065426129</v>
       </c>
       <c r="AC2">
         <f t="shared" si="0"/>
-        <v>145.30872799069601</v>
+        <v>189.66426156538949</v>
       </c>
       <c r="AD2">
         <f t="shared" si="0"/>
-        <v>141.22801890182421</v>
+        <v>185.5835524765177</v>
       </c>
       <c r="AE2">
         <f t="shared" si="0"/>
-        <v>137.14730981295241</v>
+        <v>181.5028433876459</v>
       </c>
       <c r="AF2">
         <f>'Fuhrman data'!B1*About!A25</f>
-        <v>133.06660072408053</v>
+        <v>177.42213429877404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>